<commit_message>
2D Character - Movement scripting
</commit_message>
<xml_diff>
--- a/Day 2/Assets/Orc Layers & Positon.xlsx
+++ b/Day 2/Assets/Orc Layers & Positon.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Orc</t>
   </si>
@@ -65,6 +65,48 @@
   </si>
   <si>
     <t>Player</t>
+  </si>
+  <si>
+    <t>Pivot X</t>
+  </si>
+  <si>
+    <t>Pivot Y</t>
+  </si>
+  <si>
+    <t>0.486188</t>
+  </si>
+  <si>
+    <t>0.1940409</t>
+  </si>
+  <si>
+    <t>0.6884093</t>
+  </si>
+  <si>
+    <t>0.818301</t>
+  </si>
+  <si>
+    <t>0.219031</t>
+  </si>
+  <si>
+    <t>0.8085149</t>
+  </si>
+  <si>
+    <t>0.263753</t>
+  </si>
+  <si>
+    <t>0.7673514</t>
+  </si>
+  <si>
+    <t>0.3787468</t>
+  </si>
+  <si>
+    <t>0.921729</t>
+  </si>
+  <si>
+    <t>0.3634006</t>
+  </si>
+  <si>
+    <t>0.9244167</t>
   </si>
 </sst>
 </file>
@@ -109,17 +151,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -162,16 +223,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H11" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B2:H11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B13:H22" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="B13:H22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Orc" dataDxfId="6"/>
-    <tableColumn id="2" name="Layer" dataDxfId="5"/>
-    <tableColumn id="3" name="Sorting Layer" dataDxfId="4"/>
-    <tableColumn id="4" name="Order" dataDxfId="3"/>
-    <tableColumn id="5" name="X position" dataDxfId="2"/>
-    <tableColumn id="6" name="Y position" dataDxfId="1"/>
-    <tableColumn id="7" name="Z position" dataDxfId="0"/>
+    <tableColumn id="1" name="Orc" dataDxfId="10"/>
+    <tableColumn id="2" name="Layer" dataDxfId="9"/>
+    <tableColumn id="3" name="Sorting Layer" dataDxfId="8"/>
+    <tableColumn id="4" name="Order" dataDxfId="7"/>
+    <tableColumn id="5" name="X position" dataDxfId="6"/>
+    <tableColumn id="6" name="Y position" dataDxfId="5"/>
+    <tableColumn id="7" name="Z position" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:D11" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B2:D11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Orc" dataDxfId="2"/>
+    <tableColumn id="2" name="Pivot X" dataDxfId="1"/>
+    <tableColumn id="3" name="Pivot Y" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -464,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +548,7 @@
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,22 +558,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -508,45 +569,21 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -554,22 +591,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -577,22 +602,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -600,68 +613,32 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>-0.9</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>-1.1499999999999999</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -669,22 +646,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>-0.4</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-1.4</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -692,29 +657,248 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="G11" s="2">
-        <v>-1.4</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.1458159</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-0.1245941</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1.6204050000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-0.73761379999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.18357100000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-0.46795540000000002</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-1.230647</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.5498632</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.2268070000000001E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.059995</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-1.0417620000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-1.526686E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-1.1071260000000001</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>-0.2869641</v>
+      </c>
+      <c r="G21" s="3">
+        <v>-0.9984478</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.27376739999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-1.0220290000000001</v>
+      </c>
+      <c r="H22" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>